<commit_message>
Adjustments for additional level or requirements levels
</commit_message>
<xml_diff>
--- a/data-raw/datalist_de.xlsx
+++ b/data-raw/datalist_de.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBD8920-C4B2-4285-99C7-9A9CC495409F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1C7927-78C0-490F-B77B-EDC8FA5ED7AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,20 +99,6 @@
   </si>
   <si>
     <r>
-      <t>Zulagen</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-(Schicht-, Sonntags- und Nachtarbeit sowie andere Erschwerniszulagen, 1/12 der Jahressumme)</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>13. Monatslohn</t>
     </r>
     <r>
@@ -233,6 +219,20 @@
         <family val="2"/>
       </rPr>
       <t>(gemäss Beschäftigungsgrad)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Zulagen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+(Schicht-, Sonntags- und Nachtarbeit sowie andere Erschwerniszulagen)</t>
     </r>
   </si>
 </sst>
@@ -459,9 +459,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -499,9 +499,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -534,9 +534,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -569,9 +586,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -757,7 +791,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="12"/>
     </row>
@@ -767,10 +801,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -779,7 +813,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="13">
         <v>1</v>
@@ -819,9 +853,9 @@
     <col min="19" max="23" width="8.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="213.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="218.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>11</v>
@@ -839,10 +873,10 @@
         <v>13</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>9</v>
@@ -851,22 +885,22 @@
         <v>10</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>2</v>

</xml_diff>